<commit_message>
intermidiate step for QUERY function
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4155" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="5055" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,17 +351,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="e">
+        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),1,1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="e">
+        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),1,2)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
-        <f ca="1">QUERY("SELECT * FROM PERSONS WHERE AGE = 0 OR AGE = 1 OR FIRSTNAME = '2'","pers",48,36,"Tom B.")</f>
+        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),2,1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="e">
+        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),2,2)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>

<commit_message>
QUERY function implementation with ILazyDataSet concept
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="5055" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="5505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,32 +354,32 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="e">
-        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),1,1)</f>
+        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="e">
-        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),1,2)</f>
+        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),1,2)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
-        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),2,1)</f>
+        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),2,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="e">
-        <f ca="1">INDEX(QUERY("querydefine.xlsx","pers",48,36,"Tom B."),2,2)</f>
+        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),2,2)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>

<commit_message>
demo for QUERY and DSLOOKUP is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="5505" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="6405" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,10 +351,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,6 +383,12 @@
         <v>#NAME?</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="e">
+        <f ca="1">DSLOOKUP("pers", "ADDRESS", "Abc St.", "CITY", "Lublin", "LASTNAME")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
javax.cache is now used as storage for everythind (datamodels, datasets) with no realisation in core lib
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="6855" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="7305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ehcache is added as reference implementation of jcache
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="7305" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="7755" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +385,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="e">
-        <f ca="1">DSLOOKUP("pers", "ADDRESS", "Abc St.", "CITY", "Lublin", "LASTNAME")</f>
+        <f ca="1">DSLOOKUP("pers", "ADDRESS", "Abc St.", "CITY", "Lublin", "AGE", 48, "LASTNAME")</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ITs are organized to packages and more sql data is added in demo project
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/query/query.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="7755" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="9105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,41 +351,71 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="e">
-        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),1,1)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <f ca="1">INDEX(QUERY("PersonsWithCreaditCard","pers",48,36,"Tom B."),1,1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C1" t="e">
+        <f ca="1">QUERY("AllSkills","alls")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="e">
-        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),1,2)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <f ca="1">INDEX(QUERY("PersonsWithCreaditCard","pers",48,36,"Tom B."),1,2)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C2" t="e">
+        <f ca="1">INDEX(QUERY("SkillsInCity","sodessa","Odessa"),1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
-        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),2,1)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <f ca="1">INDEX(QUERY("PersonsWithCreaditCard","pers",48,36,"Tom B."),2,1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C3" t="e">
+        <f ca="1">INDEX(QUERY("SkillsForQualification","sqa", "QA"),2,1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="e">
-        <f ca="1">INDEX(QUERY("P","pers",48,36,"Tom B."),2,2)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <f ca="1">INDEX(QUERY("PersonsWithCreaditCard","pers",48,36,"Tom B."),2,2)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C4" t="e">
+        <f ca="1">QUERY("SkillsForLevelOfEnglish","sel","5.0")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="e">
         <f ca="1">DSLOOKUP("pers", "ADDRESS", "Abc St.", "CITY", "Lublin", "AGE", 48, "LASTNAME")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C6" t="e">
+        <f ca="1">DSLOOKUP("alls", "LEVEL", "Senior", "LASTNAME")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="e">
+        <f ca="1">DSLOOKUP("sodessa", "QUALIFICATION", "QA", "LEVEL", "Middle", "FIRSTNAME")</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>